<commit_message>
Rewrite benchmark in benchmark_idep_mahdi
</commit_message>
<xml_diff>
--- a/modulation_allocations_familiales/IDEP.xlsx
+++ b/modulation_allocations_familiales/IDEP.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
-  <si>
-    <t>index</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>variable</t>
   </si>
@@ -29,6 +26,9 @@
   </si>
   <si>
     <t>Allègement sur les bas salaires (Fillon)</t>
+  </si>
+  <si>
+    <t>Crédit d'impôt compétitivité-emploi</t>
   </si>
   <si>
     <t>Salaires bruts</t>
@@ -456,13 +456,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:21">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -523,33 +523,30 @@
       <c r="U1" s="1">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
       <c r="C3" s="2">
-        <v>12106.447265625</v>
+        <v>14571.9951171875</v>
       </c>
       <c r="D3" s="2">
-        <v>26991.482421875</v>
+        <v>26044.11328125</v>
       </c>
       <c r="E3" s="2">
-        <v>45192.5390625</v>
+        <v>43771.484375</v>
       </c>
       <c r="F3" s="2">
-        <v>60211.6875</v>
+        <v>58316.94921875</v>
       </c>
       <c r="G3" s="2">
         <v>75175.703125</v>
@@ -596,19 +593,16 @@
       <c r="U3" s="2">
         <v>270725.15625</v>
       </c>
-      <c r="V3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>-4538.02490234375</v>
+        <v>-7477.2587890625</v>
       </c>
       <c r="D4" s="2">
         <v>-9075.69140625</v>
@@ -664,13 +658,10 @@
       <c r="U4" s="2">
         <v>-70725.1484375</v>
       </c>
-      <c r="V4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -732,504 +723,480 @@
       <c r="U5" s="2">
         <v>0</v>
       </c>
-      <c r="V5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>473.684204101562</v>
+      </c>
+      <c r="D6" s="2">
+        <v>947.368408203125</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1421.05285644531</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1894.73681640625</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>10526.3173828125</v>
-      </c>
-      <c r="D6" s="2">
-        <v>21052.6333007812</v>
-      </c>
-      <c r="E6" s="2">
-        <v>31578.9423828125</v>
-      </c>
-      <c r="F6" s="2">
-        <v>42105.265625</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10526.3155517578</v>
+      </c>
+      <c r="D7" s="2">
+        <v>21052.6325683594</v>
+      </c>
+      <c r="E7" s="2">
+        <v>31578.9405517578</v>
+      </c>
+      <c r="F7" s="2">
+        <v>42105.2641601562</v>
+      </c>
+      <c r="G7" s="2">
         <v>52631.580078125</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H7" s="2">
         <v>63157.888671875</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I7" s="2">
         <v>73684.2109375</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J7" s="2">
         <v>84210.53125</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K7" s="2">
         <v>94736.8359375</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L7" s="2">
         <v>105263.1484375</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M7" s="2">
         <v>115789.484375</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N7" s="2">
         <v>126315.7734375</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O7" s="2">
         <v>136842.10546875</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P7" s="2">
         <v>147368.4140625</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q7" s="2">
         <v>157894.6953125</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R7" s="2">
         <v>168421.06640625</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S7" s="2">
         <v>178947.375</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T7" s="2">
         <v>189473.6640625</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U7" s="2">
         <v>200000.0078125</v>
       </c>
-      <c r="V6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>-1478.88012695312</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-2436.84008789062</v>
+      </c>
+      <c r="D8" s="2">
         <v>-2958.1201171875</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E8" s="2">
         <v>-4436.8798828125</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>-5451.0703125</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G8" s="2">
         <v>-5903.47021484375</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H8" s="2">
         <v>-6356.33984375</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I8" s="2">
         <v>-6808.8701171875</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J8" s="2">
         <v>-7261.50048828125</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K8" s="2">
         <v>-7714.14990234375</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L8" s="2">
         <v>-8166.810546875</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M8" s="2">
         <v>-8585.48046875</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N8" s="2">
         <v>-8943.439453125</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O8" s="2">
         <v>-9301.2802734375</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P8" s="2">
         <v>-9644.8603515625</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q8" s="2">
         <v>-9812.01953125</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R8" s="2">
         <v>-9917.3798828125</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S8" s="2">
         <v>-10022.619140625</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T8" s="2">
         <v>-10127.8603515625</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U8" s="2">
         <v>-10233.2197265625</v>
       </c>
-      <c r="V7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
         <v>-527.447814941406</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>-1054.89562988281</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>-1582.34338378906</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <v>-2109.79125976562</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G9" s="2">
         <v>-2637.23999023438</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H9" s="2">
         <v>-3164.68090820312</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I9" s="2">
         <v>-3692.12963867188</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J9" s="2">
         <v>-4219.57666015625</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K9" s="2">
         <v>-4747.02490234375</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L9" s="2">
         <v>-5274.47265625</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M9" s="2">
         <v>-5801.919921875</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N9" s="2">
         <v>-6329.36767578125</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O9" s="2">
         <v>-6856.81640625</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P9" s="2">
         <v>-7384.7998046875</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q9" s="2">
         <v>-7919.328125</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R9" s="2">
         <v>-8456.1728515625</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S9" s="2">
         <v>-8993.0146484375</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T9" s="2">
         <v>-9529.857421875</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U9" s="2">
         <v>-10066.697265625</v>
       </c>
-      <c r="V8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2">
-        <v>8519.98944091797</v>
-      </c>
-      <c r="D9" s="2">
-        <v>17039.6175537109</v>
-      </c>
-      <c r="E9" s="2">
-        <v>25559.7191162109</v>
-      </c>
-      <c r="F9" s="2">
-        <v>34544.4040527344</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7562.02764892578</v>
+      </c>
+      <c r="D10" s="2">
+        <v>17039.6168212891</v>
+      </c>
+      <c r="E10" s="2">
+        <v>25559.7172851562</v>
+      </c>
+      <c r="F10" s="2">
+        <v>34544.4025878906</v>
+      </c>
+      <c r="G10" s="2">
         <v>44090.8698730469</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <v>53636.8679199219</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I10" s="2">
         <v>63183.2111816406</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J10" s="2">
         <v>72729.4541015625</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K10" s="2">
         <v>82275.6611328125</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L10" s="2">
         <v>91821.865234375</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M10" s="2">
         <v>101402.083984375</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N10" s="2">
         <v>111042.966308594</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O10" s="2">
         <v>120684.008789062</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P10" s="2">
         <v>130338.75390625</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q10" s="2">
         <v>140163.34765625</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R10" s="2">
         <v>150047.513671875</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S10" s="2">
         <v>159931.741210938</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T10" s="2">
         <v>169815.946289062</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U10" s="2">
         <v>179700.090820312</v>
       </c>
-      <c r="V9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
         <v>-248.210800170898</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="2">
         <v>-496.421600341797</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="2">
         <v>-744.632263183594</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>-992.843200683594</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G11" s="2">
         <v>-1241.05383300781</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H11" s="2">
         <v>-1489.26171875</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I11" s="2">
         <v>-1737.47277832031</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J11" s="2">
         <v>-1985.68347167969</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K11" s="2">
         <v>-2233.89404296875</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L11" s="2">
         <v>-2482.10473632812</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M11" s="2">
         <v>-2730.31616210938</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N11" s="2">
         <v>-2978.52612304688</v>
       </c>
-      <c r="O10" s="2">
+      <c r="O11" s="2">
         <v>-3226.7373046875</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P11" s="2">
         <v>-3475.19995117188</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="Q11" s="2">
         <v>-3726.7431640625</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R11" s="2">
         <v>-3979.375</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S11" s="2">
         <v>-4232.00634765625</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T11" s="2">
         <v>-4484.63818359375</v>
       </c>
-      <c r="U10" s="2">
+      <c r="U11" s="2">
         <v>-4737.26904296875</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>0</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
         <v>-51.7105827331543</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="2">
         <v>-103.421165466309</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E12" s="2">
         <v>-155.131729125977</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <v>-206.842330932617</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>-258.552917480469</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H12" s="2">
         <v>-310.262817382812</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I12" s="2">
         <v>-361.973480224609</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J12" s="2">
         <v>-413.683990478516</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K12" s="2">
         <v>-465.394653320312</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L12" s="2">
         <v>-517.105163574219</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M12" s="2">
         <v>-568.815734863281</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N12" s="2">
         <v>-620.526184082031</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O12" s="2">
         <v>-672.236938476562</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P12" s="2">
         <v>-723.999938964844</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="Q12" s="2">
         <v>-776.404968261719</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R12" s="2">
         <v>-829.036315917969</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S12" s="2">
         <v>-881.668029785156</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T12" s="2">
         <v>-934.299743652344</v>
       </c>
-      <c r="U11" s="2">
+      <c r="U12" s="2">
         <v>-986.931091308594</v>
       </c>
-      <c r="V11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>8220.06805801392</v>
-      </c>
-      <c r="D12" s="2">
-        <v>16439.7747879028</v>
-      </c>
-      <c r="E12" s="2">
-        <v>24659.9551239014</v>
-      </c>
-      <c r="F12" s="2">
-        <v>33344.7185211182</v>
-      </c>
-      <c r="G12" s="2">
-        <v>42591.2631225586</v>
-      </c>
-      <c r="H12" s="2">
-        <v>51837.3433837891</v>
-      </c>
-      <c r="I12" s="2">
-        <v>61083.7649230957</v>
-      </c>
-      <c r="J12" s="2">
-        <v>70330.0866394043</v>
-      </c>
-      <c r="K12" s="2">
-        <v>79576.3724365234</v>
-      </c>
-      <c r="L12" s="2">
-        <v>88822.6553344727</v>
-      </c>
-      <c r="M12" s="2">
-        <v>98102.9520874023</v>
-      </c>
-      <c r="N12" s="2">
-        <v>107443.914001465</v>
-      </c>
-      <c r="O12" s="2">
-        <v>116785.034545898</v>
-      </c>
-      <c r="P12" s="2">
-        <v>126139.554016113</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>135660.199523926</v>
-      </c>
-      <c r="R12" s="2">
-        <v>145239.102355957</v>
-      </c>
-      <c r="S12" s="2">
-        <v>154818.066833496</v>
-      </c>
-      <c r="T12" s="2">
-        <v>164397.008361816</v>
-      </c>
-      <c r="U12" s="2">
-        <v>173975.890686035</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B13" s="2">
         <v>0</v>
       </c>
       <c r="C13" s="2">
-        <v>8220.06805801392</v>
+        <v>7262.10626602173</v>
       </c>
       <c r="D13" s="2">
-        <v>16439.7747879028</v>
+        <v>16439.774055481</v>
       </c>
       <c r="E13" s="2">
-        <v>24659.9551239014</v>
+        <v>24659.9532928467</v>
       </c>
       <c r="F13" s="2">
-        <v>33344.7185211182</v>
+        <v>33344.7170562744</v>
       </c>
       <c r="G13" s="2">
         <v>42591.2631225586</v>
@@ -1276,28 +1243,25 @@
       <c r="U13" s="2">
         <v>173975.890686035</v>
       </c>
-      <c r="V13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>8220.06805801392</v>
+        <v>7262.10626602173</v>
       </c>
       <c r="D14" s="2">
-        <v>16439.7747879028</v>
+        <v>16439.774055481</v>
       </c>
       <c r="E14" s="2">
-        <v>24659.9551239014</v>
+        <v>24659.9532928467</v>
       </c>
       <c r="F14" s="2">
-        <v>33344.7185211182</v>
+        <v>33344.7170562744</v>
       </c>
       <c r="G14" s="2">
         <v>42591.2631225586</v>
@@ -1344,960 +1308,980 @@
       <c r="U14" s="2">
         <v>173975.890686035</v>
       </c>
-      <c r="V14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>7262.10626602173</v>
+      </c>
+      <c r="D15" s="2">
+        <v>16439.774055481</v>
+      </c>
+      <c r="E15" s="2">
+        <v>24659.9532928467</v>
+      </c>
+      <c r="F15" s="2">
+        <v>33344.7170562744</v>
+      </c>
+      <c r="G15" s="2">
+        <v>42591.2631225586</v>
+      </c>
+      <c r="H15" s="2">
+        <v>51837.3433837891</v>
+      </c>
+      <c r="I15" s="2">
+        <v>61083.7649230957</v>
+      </c>
+      <c r="J15" s="2">
+        <v>70330.0866394043</v>
+      </c>
+      <c r="K15" s="2">
+        <v>79576.3724365234</v>
+      </c>
+      <c r="L15" s="2">
+        <v>88822.6553344727</v>
+      </c>
+      <c r="M15" s="2">
+        <v>98102.9520874023</v>
+      </c>
+      <c r="N15" s="2">
+        <v>107443.914001465</v>
+      </c>
+      <c r="O15" s="2">
+        <v>116785.034545898</v>
+      </c>
+      <c r="P15" s="2">
+        <v>126139.554016113</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>135660.199523926</v>
+      </c>
+      <c r="R15" s="2">
+        <v>145239.102355957</v>
+      </c>
+      <c r="S15" s="2">
+        <v>154818.066833496</v>
+      </c>
+      <c r="T15" s="2">
+        <v>164397.008361816</v>
+      </c>
+      <c r="U15" s="2">
+        <v>173975.890686035</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B16" s="2">
         <v>1557.53991699219</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C16" s="2">
         <v>1557.5400390625</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="2">
         <v>1557.53979492188</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <v>1557.53979492188</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>1557.53979492188</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="2">
         <v>1557.53979492188</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H16" s="2">
         <v>1557.54052734375</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I16" s="2">
         <v>1557.5419921875</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J16" s="2">
         <v>1557.5419921875</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K16" s="2">
         <v>778.77099609375</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L16" s="2">
         <v>778.77099609375</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M16" s="2">
         <v>778.77099609375</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="O15" s="2">
+      <c r="O16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U16" s="2">
         <v>389.3818359375</v>
       </c>
-      <c r="V15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="Q17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S17" s="2">
         <v>724.560791015625</v>
       </c>
-      <c r="T16" s="2">
-        <v>0</v>
-      </c>
-      <c r="U16" s="2">
-        <v>0</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
-      <c r="A17" s="1" t="s">
+      <c r="T17" s="2">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="2">
         <v>-11.4105024337769</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C18" s="2">
         <v>-11.4105043411255</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="2">
         <v>-11.4105024337769</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E18" s="2">
         <v>-11.4105024337769</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <v>-11.4105024337769</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G18" s="2">
         <v>-11.4105024337769</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H18" s="2">
         <v>-11.4105062484741</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I18" s="2">
         <v>-11.4105138778687</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J18" s="2">
         <v>-11.4105138778687</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K18" s="2">
         <v>-7.51665878295898</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L18" s="2">
         <v>-7.51665878295898</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M18" s="2">
         <v>-7.51665878295898</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N18" s="2">
         <v>-5.56971311569214</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O18" s="2">
         <v>-5.56971311569214</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P18" s="2">
         <v>-5.56971311569214</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="Q18" s="2">
         <v>-5.56971311569214</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R18" s="2">
         <v>-5.56971311569214</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S18" s="2">
         <v>-5.56971311569214</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T18" s="2">
         <v>-1.94690918922424</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U18" s="2">
         <v>-1.94690918922424</v>
       </c>
-      <c r="V17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22">
-      <c r="A18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <v>2270.69020557404</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>2270.690325737</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>2270.69008350372</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="2">
         <v>2270.69008350372</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="2">
         <v>2270.69008350372</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G19" s="2">
         <v>2270.69008350372</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H19" s="2">
         <v>2270.6908121109</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I19" s="2">
         <v>2270.69226932526</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J19" s="2">
         <v>2270.69226932526</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K19" s="2">
         <v>1495.81512832642</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L19" s="2">
         <v>1495.81512832642</v>
       </c>
-      <c r="M18" s="2">
+      <c r="M19" s="2">
         <v>1495.81512832642</v>
       </c>
-      <c r="N18" s="2">
+      <c r="N19" s="2">
         <v>1108.37291383743</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O19" s="2">
         <v>1108.37291383743</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P19" s="2">
         <v>1108.37291383743</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q19" s="2">
         <v>1108.37291383743</v>
       </c>
-      <c r="R18" s="2">
+      <c r="R19" s="2">
         <v>1108.37291383743</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S19" s="2">
         <v>1108.37291383743</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T19" s="2">
         <v>387.434926748276</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U19" s="2">
         <v>387.434926748276</v>
       </c>
-      <c r="V18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="2">
         <v>9317.580078125</v>
       </c>
-      <c r="C19" s="2">
-        <v>6714.5576171875</v>
-      </c>
-      <c r="D19" s="2">
+      <c r="C20" s="2">
+        <v>7017.912109375</v>
+      </c>
+      <c r="D20" s="2">
         <v>4111.65185546875</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2">
         <v>1561.75708007812</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>1257.22180175781</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G20" s="2">
         <v>1092.517578125</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H20" s="2">
         <v>994.920043945312</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I20" s="2">
         <v>897.319030761719</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J20" s="2">
         <v>799.718811035156</v>
       </c>
-      <c r="K19" s="2">
+      <c r="K20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="Q20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U20" s="2">
         <v>771.045959472656</v>
       </c>
-      <c r="V19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U21" s="2">
         <v>320.144989013672</v>
       </c>
-      <c r="V20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22">
-      <c r="A21" s="1" t="s">
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="2">
         <v>9637.72506713867</v>
       </c>
-      <c r="C21" s="2">
-        <v>7034.70260620117</v>
-      </c>
-      <c r="D21" s="2">
+      <c r="C22" s="2">
+        <v>7338.05709838867</v>
+      </c>
+      <c r="D22" s="2">
         <v>4431.79684448242</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E22" s="2">
         <v>1881.9020690918</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>1577.36679077148</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G22" s="2">
         <v>1412.66256713867</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H22" s="2">
         <v>1315.06503295898</v>
       </c>
-      <c r="I21" s="2">
+      <c r="I22" s="2">
         <v>1217.46401977539</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J22" s="2">
         <v>1119.86380004883</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="Q22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="U21" s="2">
+      <c r="U22" s="2">
         <v>1091.19094848633</v>
       </c>
-      <c r="V21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22">
-      <c r="A22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="N22" s="2">
+      <c r="N23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="Q23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="R22" s="2">
+      <c r="R23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="S22" s="2">
+      <c r="S23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="U22" s="2">
+      <c r="U23" s="2">
         <v>1508.56018066406</v>
       </c>
-      <c r="V22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22">
-      <c r="A23" s="1" t="s">
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="Q24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="R23" s="2">
+      <c r="R24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="T23" s="2">
+      <c r="T24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="U23" s="2">
+      <c r="U24" s="2">
         <v>-7.54280042648315</v>
       </c>
-      <c r="V23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22">
-      <c r="A24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="N24" s="2">
+      <c r="N25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="O24" s="2">
+      <c r="O25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="P24" s="2">
+      <c r="P25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="Q24" s="2">
+      <c r="Q25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="R24" s="2">
+      <c r="R25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="S24" s="2">
+      <c r="S25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="T24" s="2">
+      <c r="T25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="U24" s="2">
+      <c r="U25" s="2">
         <v>1501.01738023758</v>
       </c>
-      <c r="V24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22">
-      <c r="A25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="2">
         <v>13409.4326529503</v>
       </c>
-      <c r="C25" s="2">
-        <v>10806.4103121758</v>
-      </c>
-      <c r="D25" s="2">
+      <c r="C26" s="2">
+        <v>11109.7648043633</v>
+      </c>
+      <c r="D26" s="2">
         <v>8203.50430822372</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E26" s="2">
         <v>5653.6095328331</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F26" s="2">
         <v>5349.07425451279</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G26" s="2">
         <v>5184.37003087997</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H26" s="2">
         <v>5086.77322530746</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I26" s="2">
         <v>4989.17366933823</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J26" s="2">
         <v>4891.57344961166</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K26" s="2">
         <v>4088.02345705032</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L26" s="2">
         <v>4088.02345705032</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M26" s="2">
         <v>4088.02345705032</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N26" s="2">
         <v>3700.58124256134</v>
       </c>
-      <c r="O25" s="2">
+      <c r="O26" s="2">
         <v>3700.58124256134</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P26" s="2">
         <v>3700.58124256134</v>
       </c>
-      <c r="Q25" s="2">
+      <c r="Q26" s="2">
         <v>3700.58124256134</v>
       </c>
-      <c r="R25" s="2">
+      <c r="R26" s="2">
         <v>3700.58124256134</v>
       </c>
-      <c r="S25" s="2">
+      <c r="S26" s="2">
         <v>3700.58124256134</v>
       </c>
-      <c r="T25" s="2">
+      <c r="T26" s="2">
         <v>2979.64325547218</v>
       </c>
-      <c r="U25" s="2">
+      <c r="U26" s="2">
         <v>2979.64325547218</v>
       </c>
-      <c r="V25" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26" s="1" t="s">
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
-        <v>0</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>-250.480926513672</v>
-      </c>
-      <c r="F26" s="2">
-        <v>-1639.45629882812</v>
-      </c>
-      <c r="G26" s="2">
-        <v>-3249.72119140625</v>
-      </c>
-      <c r="H26" s="2">
-        <v>-5827.0205078125</v>
-      </c>
-      <c r="I26" s="2">
-        <v>-8404.7216796875</v>
-      </c>
-      <c r="J26" s="2">
-        <v>-10982.095703125</v>
-      </c>
-      <c r="K26" s="2">
-        <v>-13811.76171875</v>
-      </c>
-      <c r="L26" s="2">
-        <v>-17334.568359375</v>
-      </c>
-      <c r="M26" s="2">
-        <v>-20869.677734375</v>
-      </c>
-      <c r="N26" s="2">
-        <v>-24427.197265625</v>
-      </c>
-      <c r="O26" s="2">
-        <v>-27984.787109375</v>
-      </c>
-      <c r="P26" s="2">
-        <v>-31931.34375</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>-35959.42578125</v>
-      </c>
-      <c r="R26" s="2">
-        <v>-40011.9296875</v>
-      </c>
-      <c r="S26" s="2">
-        <v>-44064.4609375</v>
-      </c>
-      <c r="T26" s="2">
-        <v>-48377.75</v>
-      </c>
-      <c r="U26" s="2">
-        <v>-52825.61328125</v>
-      </c>
-      <c r="V26" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>-390.541778564453</v>
+      </c>
+      <c r="F27" s="2">
+        <v>-1639.47631835938</v>
+      </c>
+      <c r="G27" s="2">
+        <v>-3265.7314453125</v>
+      </c>
+      <c r="H27" s="2">
+        <v>-5843.0302734375</v>
+      </c>
+      <c r="I27" s="2">
+        <v>-8420.732421875</v>
+      </c>
+      <c r="J27" s="2">
+        <v>-10998.10546875</v>
+      </c>
+      <c r="K27" s="2">
+        <v>-13827.771484375</v>
+      </c>
+      <c r="L27" s="2">
+        <v>-17350.578125</v>
+      </c>
+      <c r="M27" s="2">
+        <v>-20885.6875</v>
+      </c>
+      <c r="N27" s="2">
+        <v>-24443.20703125</v>
+      </c>
+      <c r="O27" s="2">
+        <v>-28000.796875</v>
+      </c>
+      <c r="P27" s="2">
+        <v>-31947.35546875</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>-35975.4375</v>
+      </c>
+      <c r="R27" s="2">
+        <v>-40027.94140625</v>
+      </c>
+      <c r="S27" s="2">
+        <v>-44080.47265625</v>
+      </c>
+      <c r="T27" s="2">
+        <v>-48363.51953125</v>
+      </c>
+      <c r="U27" s="2">
+        <v>-52811.3828125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
-        <v>0</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>-250.480926513672</v>
-      </c>
-      <c r="F27" s="2">
-        <v>-1639.45629882812</v>
-      </c>
-      <c r="G27" s="2">
-        <v>-3249.72119140625</v>
-      </c>
-      <c r="H27" s="2">
-        <v>-5827.0205078125</v>
-      </c>
-      <c r="I27" s="2">
-        <v>-8404.7216796875</v>
-      </c>
-      <c r="J27" s="2">
-        <v>-10982.095703125</v>
-      </c>
-      <c r="K27" s="2">
-        <v>-13811.76171875</v>
-      </c>
-      <c r="L27" s="2">
-        <v>-17334.568359375</v>
-      </c>
-      <c r="M27" s="2">
-        <v>-20869.677734375</v>
-      </c>
-      <c r="N27" s="2">
-        <v>-24427.197265625</v>
-      </c>
-      <c r="O27" s="2">
-        <v>-27984.787109375</v>
-      </c>
-      <c r="P27" s="2">
-        <v>-31931.34375</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>-35959.42578125</v>
-      </c>
-      <c r="R27" s="2">
-        <v>-40011.9296875</v>
-      </c>
-      <c r="S27" s="2">
-        <v>-44064.4609375</v>
-      </c>
-      <c r="T27" s="2">
-        <v>-48377.75</v>
-      </c>
-      <c r="U27" s="2">
-        <v>-52825.61328125</v>
-      </c>
-      <c r="V27" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="2">
+        <v>0</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>-390.541778564453</v>
+      </c>
+      <c r="F28" s="2">
+        <v>-1639.47631835938</v>
+      </c>
+      <c r="G28" s="2">
+        <v>-3265.7314453125</v>
+      </c>
+      <c r="H28" s="2">
+        <v>-5843.0302734375</v>
+      </c>
+      <c r="I28" s="2">
+        <v>-8420.732421875</v>
+      </c>
+      <c r="J28" s="2">
+        <v>-10998.10546875</v>
+      </c>
+      <c r="K28" s="2">
+        <v>-13827.771484375</v>
+      </c>
+      <c r="L28" s="2">
+        <v>-17350.578125</v>
+      </c>
+      <c r="M28" s="2">
+        <v>-20885.6875</v>
+      </c>
+      <c r="N28" s="2">
+        <v>-24443.20703125</v>
+      </c>
+      <c r="O28" s="2">
+        <v>-28000.796875</v>
+      </c>
+      <c r="P28" s="2">
+        <v>-31947.35546875</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>-35975.4375</v>
+      </c>
+      <c r="R28" s="2">
+        <v>-40027.94140625</v>
+      </c>
+      <c r="S28" s="2">
+        <v>-44080.47265625</v>
+      </c>
+      <c r="T28" s="2">
+        <v>-48363.51953125</v>
+      </c>
+      <c r="U28" s="2">
+        <v>-52811.3828125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="2">
         <v>13409.4326529503</v>
       </c>
-      <c r="C28" s="2">
-        <v>19026.4783701897</v>
-      </c>
-      <c r="D28" s="2">
-        <v>24643.2790961266</v>
-      </c>
-      <c r="E28" s="2">
-        <v>30063.0837302208</v>
-      </c>
-      <c r="F28" s="2">
-        <v>37054.3364768028</v>
-      </c>
-      <c r="G28" s="2">
-        <v>44525.9119620323</v>
-      </c>
-      <c r="H28" s="2">
-        <v>51097.096101284</v>
-      </c>
-      <c r="I28" s="2">
-        <v>57668.2169127464</v>
-      </c>
-      <c r="J28" s="2">
-        <v>64239.564385891</v>
-      </c>
-      <c r="K28" s="2">
-        <v>69852.6341748238</v>
-      </c>
-      <c r="L28" s="2">
-        <v>75576.110432148</v>
-      </c>
-      <c r="M28" s="2">
-        <v>81321.2978100777</v>
-      </c>
-      <c r="N28" s="2">
-        <v>86717.2979784012</v>
-      </c>
-      <c r="O28" s="2">
-        <v>92500.8286790848</v>
-      </c>
-      <c r="P28" s="2">
-        <v>97908.7915086746</v>
-      </c>
-      <c r="Q28" s="2">
-        <v>103401.354985237</v>
-      </c>
-      <c r="R28" s="2">
-        <v>108927.753911018</v>
-      </c>
-      <c r="S28" s="2">
-        <v>114454.187138557</v>
-      </c>
-      <c r="T28" s="2">
-        <v>118998.901617289</v>
-      </c>
-      <c r="U28" s="2">
-        <v>124129.920660257</v>
-      </c>
-      <c r="V28" s="2" t="s">
-        <v>27</v>
+      <c r="C29" s="2">
+        <v>18371.871070385</v>
+      </c>
+      <c r="D29" s="2">
+        <v>24643.2783637047</v>
+      </c>
+      <c r="E29" s="2">
+        <v>29923.0210471153</v>
+      </c>
+      <c r="F29" s="2">
+        <v>37054.3149924278</v>
+      </c>
+      <c r="G29" s="2">
+        <v>44509.9017081261</v>
+      </c>
+      <c r="H29" s="2">
+        <v>51081.086335659</v>
+      </c>
+      <c r="I29" s="2">
+        <v>57652.2061705589</v>
+      </c>
+      <c r="J29" s="2">
+        <v>64223.554620266</v>
+      </c>
+      <c r="K29" s="2">
+        <v>69836.6244091988</v>
+      </c>
+      <c r="L29" s="2">
+        <v>75560.100666523</v>
+      </c>
+      <c r="M29" s="2">
+        <v>81305.2880444527</v>
+      </c>
+      <c r="N29" s="2">
+        <v>86701.2882127762</v>
+      </c>
+      <c r="O29" s="2">
+        <v>92484.8189134598</v>
+      </c>
+      <c r="P29" s="2">
+        <v>97892.7797899246</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>103385.343266487</v>
+      </c>
+      <c r="R29" s="2">
+        <v>108911.742192268</v>
+      </c>
+      <c r="S29" s="2">
+        <v>114438.175419807</v>
+      </c>
+      <c r="T29" s="2">
+        <v>119013.132086039</v>
+      </c>
+      <c r="U29" s="2">
+        <v>124144.151129007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>